<commit_message>
b negativo y algunas cosas mas
</commit_message>
<xml_diff>
--- a/posiciones_PU300.xlsx
+++ b/posiciones_PU300.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdmed\Downloads\TemporalUniandes\SextoSemestre\Análisis_Inteligente_De_Señales_Y_Sistemas\ProyectoFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FADD698-5A99-4345-BEAF-E43622CCEDBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387DDBDC-3ECB-496A-A4B0-1B9039BF76B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -361,8 +361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,7 +388,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>4.0999999999999996</v>
+        <v>4.5</v>
       </c>
       <c r="B3" s="1">
         <v>5.25</v>
@@ -396,7 +396,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>4.0999999999999996</v>
+        <v>4.5</v>
       </c>
       <c r="B4" s="1">
         <f>B3-1.1</f>
@@ -405,7 +405,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>4.0999999999999996</v>
+        <v>4.5</v>
       </c>
       <c r="B5" s="1">
         <f t="shared" ref="B5:B6" si="0">B4-1.1</f>
@@ -414,7 +414,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>4.0999999999999996</v>
+        <v>4.5</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" si="0"/>
@@ -423,7 +423,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>4.0999999999999996</v>
+        <v>4.5</v>
       </c>
       <c r="B7" s="1">
         <v>0.1</v>
@@ -431,7 +431,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>3.1</v>
+        <v>3.6</v>
       </c>
       <c r="B8" s="1">
         <v>5.25</v>
@@ -439,7 +439,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>3.1</v>
+        <v>3.6</v>
       </c>
       <c r="B9" s="1">
         <f>B8-1.1</f>
@@ -448,7 +448,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>3.1</v>
+        <v>3.6</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" ref="B10:B11" si="1">B9-1.1</f>
@@ -458,7 +458,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>3.1</v>
+        <v>3.6</v>
       </c>
       <c r="B11" s="1">
         <f t="shared" si="1"/>
@@ -467,7 +467,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>3.1</v>
+        <v>3.6</v>
       </c>
       <c r="B12" s="1">
         <v>0.1</v>
@@ -475,7 +475,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>2.1</v>
+        <v>2.7</v>
       </c>
       <c r="B13" s="1">
         <v>5.25</v>
@@ -483,7 +483,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>2.1</v>
+        <v>2.7</v>
       </c>
       <c r="B14" s="1">
         <f>B13-1.1</f>
@@ -492,7 +492,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>2.1</v>
+        <v>2.7</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" ref="B15:B16" si="2">B14-1.1</f>
@@ -501,7 +501,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>2.1</v>
+        <v>2.7</v>
       </c>
       <c r="B16" s="1">
         <f t="shared" si="2"/>
@@ -510,7 +510,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>2.1</v>
+        <v>2.7</v>
       </c>
       <c r="B17" s="1">
         <v>0.1</v>
@@ -518,7 +518,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>1.1000000000000001</v>
+        <v>1.8</v>
       </c>
       <c r="B18" s="1">
         <v>5.25</v>
@@ -526,7 +526,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>1.1000000000000001</v>
+        <v>1.8</v>
       </c>
       <c r="B19" s="1">
         <f>B18-1.1</f>
@@ -535,7 +535,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>1.1000000000000001</v>
+        <v>1.8</v>
       </c>
       <c r="B20" s="1">
         <f t="shared" ref="B20:B21" si="3">B19-1.1</f>
@@ -544,7 +544,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>1.1000000000000001</v>
+        <v>1.8</v>
       </c>
       <c r="B21" s="1">
         <f t="shared" si="3"/>
@@ -553,7 +553,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>1.1000000000000001</v>
+        <v>1.8</v>
       </c>
       <c r="B22" s="1">
         <v>0.1</v>

</xml_diff>